<commit_message>
Agregar espacio para comentario en el reporte de compromisos
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluaciondeDesempenoCompTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluaciondeDesempenoCompTemplate.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teto\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755"/>
   </bookViews>
@@ -10,11 +15,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$33</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Módulo de Evaluación de Desempeño</t>
   </si>
@@ -64,16 +69,19 @@
   </si>
   <si>
     <t>Fecha de Revision de Compromisos</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +140,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -147,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -268,11 +284,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -297,49 +357,6 @@
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -366,43 +383,105 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,22 +755,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:J8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
@@ -707,37 +786,37 @@
     <col min="12" max="12" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="40" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -749,311 +828,311 @@
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="41" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="41"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="H4" s="26"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="41" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-    </row>
-    <row r="6" spans="1:12" ht="30" customHeight="1">
+      <c r="H5" s="26"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="43"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="H6" s="27"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="47" t="s">
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
       <c r="K8" s="4"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
       <c r="K9" s="4"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="32"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="21"/>
       <c r="K10" s="4"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="32"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="21"/>
       <c r="K11" s="4"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="35"/>
+    <row r="12" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
       <c r="K12" s="4"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="27"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="29"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="18"/>
       <c r="K13" s="4"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="32"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="21"/>
       <c r="K14" s="4"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="32"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="4"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="35"/>
+    <row r="16" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="24"/>
       <c r="K16" s="4"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="29"/>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="18"/>
       <c r="K17" s="4"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="20"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="32"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="35"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
       <c r="K18" s="4"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="20"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="32"/>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21"/>
       <c r="K19" s="4"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="35"/>
+    <row r="20" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="24"/>
       <c r="K20" s="4"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
       <c r="K21" s="4"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
       <c r="K22" s="4"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
       <c r="K23" s="4"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
+    <row r="24" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="4"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1065,125 +1144,194 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="10"/>
-      <c r="B27" s="38" t="s">
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="51"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="54"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="38" t="s">
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="7"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="13" t="s">
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B33" s="14">
         <f ca="1">NOW()</f>
-        <v>41887.88486377315</v>
-      </c>
-      <c r="C29" s="15">
+        <v>41907.867803587964</v>
+      </c>
+      <c r="C33" s="15">
         <f ca="1">NOW()</f>
-        <v>41887.88486377315</v>
-      </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="2"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.75">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="33" spans="2:9">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-    </row>
-    <row r="34" spans="2:9">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="2:9">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="2:9">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
+        <v>41907.867803587964</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="32">
+  <mergeCells count="33">
+    <mergeCell ref="F21:J24"/>
+    <mergeCell ref="A17:E20"/>
+    <mergeCell ref="A21:E24"/>
+    <mergeCell ref="F17:J20"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B27:J28"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D4:F4"/>
     <mergeCell ref="A13:E16"/>
     <mergeCell ref="F13:J16"/>
     <mergeCell ref="A8:E8"/>
@@ -1198,24 +1346,6 @@
     <mergeCell ref="A9:E12"/>
     <mergeCell ref="F9:J12"/>
     <mergeCell ref="D5:F5"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="F21:J24"/>
-    <mergeCell ref="A17:E20"/>
-    <mergeCell ref="A21:E24"/>
-    <mergeCell ref="F17:J20"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="B27:E27"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
En el Reporte de Compromisos ED se agrega el campo Comentarios
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluaciondeDesempenoCompTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluaciondeDesempenoCompTemplate.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teto\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755"/>
   </bookViews>
@@ -10,11 +15,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$33</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Módulo de Evaluación de Desempeño</t>
   </si>
@@ -64,16 +69,19 @@
   </si>
   <si>
     <t>Fecha de Revision de Compromisos</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +140,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -147,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -268,11 +284,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -297,49 +357,6 @@
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -366,43 +383,105 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,22 +755,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:J8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
@@ -707,37 +786,37 @@
     <col min="12" max="12" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="40" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -749,311 +828,311 @@
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="41" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="41"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="H4" s="26"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="41" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-    </row>
-    <row r="6" spans="1:12" ht="30" customHeight="1">
+      <c r="H5" s="26"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="43"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="H6" s="27"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="47" t="s">
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
       <c r="K8" s="4"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
       <c r="K9" s="4"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="32"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="21"/>
       <c r="K10" s="4"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="32"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="21"/>
       <c r="K11" s="4"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="35"/>
+    <row r="12" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
       <c r="K12" s="4"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="27"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="29"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="18"/>
       <c r="K13" s="4"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="32"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="21"/>
       <c r="K14" s="4"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="32"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="4"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="35"/>
+    <row r="16" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="24"/>
       <c r="K16" s="4"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="29"/>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="18"/>
       <c r="K17" s="4"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="20"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="32"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="35"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
       <c r="K18" s="4"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="20"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="32"/>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21"/>
       <c r="K19" s="4"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="35"/>
+    <row r="20" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="24"/>
       <c r="K20" s="4"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
       <c r="K21" s="4"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
       <c r="K22" s="4"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
       <c r="K23" s="4"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
+    <row r="24" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="4"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1065,125 +1144,194 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="10"/>
-      <c r="B27" s="38" t="s">
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="51"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="54"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="38" t="s">
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="7"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="13" t="s">
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B33" s="14">
         <f ca="1">NOW()</f>
-        <v>41887.88486377315</v>
-      </c>
-      <c r="C29" s="15">
+        <v>41907.867803587964</v>
+      </c>
+      <c r="C33" s="15">
         <f ca="1">NOW()</f>
-        <v>41887.88486377315</v>
-      </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="2"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.75">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="33" spans="2:9">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-    </row>
-    <row r="34" spans="2:9">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="2:9">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="2:9">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
+        <v>41907.867803587964</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="32">
+  <mergeCells count="33">
+    <mergeCell ref="F21:J24"/>
+    <mergeCell ref="A17:E20"/>
+    <mergeCell ref="A21:E24"/>
+    <mergeCell ref="F17:J20"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B27:J28"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D4:F4"/>
     <mergeCell ref="A13:E16"/>
     <mergeCell ref="F13:J16"/>
     <mergeCell ref="A8:E8"/>
@@ -1198,24 +1346,6 @@
     <mergeCell ref="A9:E12"/>
     <mergeCell ref="F9:J12"/>
     <mergeCell ref="D5:F5"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="F21:J24"/>
-    <mergeCell ref="A17:E20"/>
-    <mergeCell ref="A21:E24"/>
-    <mergeCell ref="F17:J20"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="B27:E27"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>